<commit_message>
excel read by coded
</commit_message>
<xml_diff>
--- a/merceria.xlsx
+++ b/merceria.xlsx
@@ -496,7 +496,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:C8"/>
   </ignoredErrors>
@@ -692,7 +691,7 @@
         <v>prov_1759546032622</v>
       </c>
       <c r="B2" t="str">
-        <v>chancho7sa</v>
+        <v>chancho77</v>
       </c>
       <c r="C2" t="str">
         <v>45646545456</v>
@@ -894,7 +893,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:I1"/>
   </ignoredErrors>
@@ -935,7 +933,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:H1"/>
   </ignoredErrors>

</xml_diff>